<commit_message>
Fiscal 16, 17, 18 & 19 for £PIER
</commit_message>
<xml_diff>
--- a/Overview - Leisure Facilities.xlsx
+++ b/Overview - Leisure Facilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E3C9AA-FEE9-4BE7-9512-48A60632E6DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1A36CC-B202-4F06-AE36-ADBC47E11E11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5EB38F2A-A5E5-4604-9A50-AFDB2AF73DAE}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Ticker</t>
   </si>
@@ -186,6 +187,45 @@
   </si>
   <si>
     <t>Cinema Chains</t>
+  </si>
+  <si>
+    <t>$SIX</t>
+  </si>
+  <si>
+    <t>Six Flags Entertainment Corporation</t>
+  </si>
+  <si>
+    <t>£GYM</t>
+  </si>
+  <si>
+    <t>The Gym Group Plc.</t>
+  </si>
+  <si>
+    <t>$PLNT</t>
+  </si>
+  <si>
+    <t>Planet Fitness Inc.</t>
+  </si>
+  <si>
+    <t>NYSE</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>£PIER</t>
+  </si>
+  <si>
+    <t>Brighton Pier Group Plc.</t>
+  </si>
+  <si>
+    <t>AIM</t>
+  </si>
+  <si>
+    <t>Pleasure Pier, Arcade &amp; MIniGolf</t>
+  </si>
+  <si>
+    <t>Brighton Pier, Lightwater Valley Theme Park &amp; more</t>
   </si>
 </sst>
 </file>
@@ -246,7 +286,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -336,6 +382,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -362,151 +430,172 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Historical Projections"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3" t="str">
-            <v>Ten Entertainment Group Plc</v>
+            <v>Hollywood Bowl Group Plc</v>
           </cell>
         </row>
         <row r="6">
           <cell r="C6">
-            <v>2.7210000000000001</v>
+            <v>2.3650000000000002</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>68.381495999999999</v>
+            <v>170.949286</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>186.06605061600001</v>
+            <v>404.29506139000006</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-200.21699999999998</v>
+            <v>56.066000000000003</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>386.28305061599997</v>
+            <v>348.22906139000008</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Cranfield, UK</v>
+            <v>Hemel, UK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>2009</v>
+            <v>2010</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>48</v>
+            <v>64</v>
           </cell>
         </row>
         <row r="26">
           <cell r="C26">
-            <v>1500</v>
+            <v>2530</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>2017</v>
+            <v>2016</v>
           </cell>
         </row>
         <row r="28">
           <cell r="C28" t="str">
-            <v>H122</v>
+            <v>FY22</v>
           </cell>
           <cell r="D28">
-            <v>45190</v>
+            <v>44911</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33">
-            <v>3.5367722369936718</v>
+            <v>3.0577866054115437</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>1.5486275426012701</v>
+            <v>5.6247399954088877</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>3.215033421967723</v>
+            <v>1.7973947764799401</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>5.9823787638134727</v>
+            <v>2.2528786210358729</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>12.421475677406907</v>
+            <v>9.2982580275560043</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="12">
+          <cell r="R12">
+            <v>18.783999999999999</v>
+          </cell>
+          <cell r="S12">
+            <v>22.285</v>
+          </cell>
+          <cell r="T12">
+            <v>1.3850000000000033</v>
+          </cell>
+          <cell r="U12">
+            <v>1.7280000000000051</v>
+          </cell>
+          <cell r="V12">
+            <v>37.451000000000015</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="V16">
+            <v>0.84829230777171583</v>
+          </cell>
+          <cell r="AO16">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="V17">
+            <v>0.28620168162650139</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="V18">
+            <v>0.19330446317506367</v>
+          </cell>
+        </row>
         <row r="19">
-          <cell r="P19">
-            <v>8.1420000000000101</v>
-          </cell>
-          <cell r="Q19">
-            <v>9.036999999999999</v>
-          </cell>
-          <cell r="R19">
-            <v>-17.747</v>
-          </cell>
-          <cell r="S19">
-            <v>4.005000000000007</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="K23">
-            <v>4.9602262016965133</v>
-          </cell>
-          <cell r="P23">
-            <v>7.4746621621621712E-2</v>
-          </cell>
-          <cell r="Q23">
-            <v>0.10179436804191222</v>
-          </cell>
-          <cell r="R23">
-            <v>-0.56885238106559521</v>
-          </cell>
-          <cell r="S23">
-            <v>0.86167250268824636</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="K26">
-            <v>0.68836775356589386</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="K27">
-            <v>0.38816850627787092</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="K28">
-            <v>0.2892880862772384</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="K29">
-            <v>5.0590924103622523E-3</v>
+          <cell r="V19">
+            <v>0.19744990892531872</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AO20">
+            <v>9.417179548242931</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="M21">
+            <v>0.5227927414761171</v>
+          </cell>
+          <cell r="R21">
+            <v>5.7735504703074536E-2</v>
+          </cell>
+          <cell r="S21">
+            <v>7.7529282941235067E-2</v>
+          </cell>
+          <cell r="T21">
+            <v>-0.38817035428888169</v>
+          </cell>
+          <cell r="U21">
+            <v>-9.5567047928227233E-2</v>
+          </cell>
+          <cell r="V21">
+            <v>1.6954144522663404</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="AO22">
+            <v>2.9818941007369681</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -523,59 +612,146 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3" t="str">
-            <v>Cineworld Group Plc.</v>
+            <v>Ten Entertainment Group Plc</v>
           </cell>
         </row>
         <row r="6">
           <cell r="C6">
-            <v>2.7E-2</v>
+            <v>2.7210000000000001</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>1370</v>
+            <v>68.381495999999999</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>36.99</v>
+            <v>186.06605061600001</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-4013.2990000000004</v>
+            <v>-200.21699999999998</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>4050.2890000000002</v>
+            <v>386.28305061599997</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Brentford, UK</v>
+            <v>Cranfield, UK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1995</v>
+            <v>2009</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>48</v>
           </cell>
         </row>
         <row r="26">
           <cell r="C26">
-            <v>751</v>
+            <v>1500</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="C27" t="str">
-            <v>FY21</v>
-          </cell>
-          <cell r="D27">
-            <v>44287</v>
+          <cell r="C27">
+            <v>2017</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28" t="str">
+            <v>H122</v>
+          </cell>
+          <cell r="D28">
+            <v>45190</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>3.5367722369936718</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>1.5486275426012701</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>3.215033421967723</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>5.9823787638134727</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>12.421475677406907</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="19">
+          <cell r="P19">
+            <v>8.1420000000000101</v>
+          </cell>
+          <cell r="Q19">
+            <v>9.036999999999999</v>
+          </cell>
+          <cell r="R19">
+            <v>-17.747</v>
+          </cell>
+          <cell r="S19">
+            <v>4.005000000000007</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="K23">
+            <v>4.9602262016965133</v>
+          </cell>
+          <cell r="P23">
+            <v>7.4746621621621712E-2</v>
+          </cell>
+          <cell r="Q23">
+            <v>0.10179436804191222</v>
+          </cell>
+          <cell r="R23">
+            <v>-0.56885238106559521</v>
+          </cell>
+          <cell r="S23">
+            <v>0.86167250268824636</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="K26">
+            <v>0.68836775356589386</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="K27">
+            <v>0.38816850627787092</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="K28">
+            <v>0.2892880862772384</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="K29">
+            <v>5.0590924103622523E-3</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -587,172 +763,202 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
-      <sheetName val="Historical Projections"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3" t="str">
-            <v>Hollywood Bowl Group Plc</v>
+            <v>Cineworld Group Plc.</v>
           </cell>
         </row>
         <row r="6">
           <cell r="C6">
-            <v>2.3650000000000002</v>
+            <v>2.7E-2</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>170.949286</v>
+            <v>1370</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>404.29506139000006</v>
+            <v>36.99</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>56.066000000000003</v>
+            <v>-4013.2990000000004</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>348.22906139000008</v>
+            <v>4050.2890000000002</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Hemel, UK</v>
+            <v>Brentford, UK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>2010</v>
+            <v>1995</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26">
+            <v>751</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>FY21</v>
+          </cell>
+          <cell r="D27">
+            <v>44287</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>0.61</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>37.286000000000001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>22.74446</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>-4.9880000000000013</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>27.732460000000003</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>London, UK</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>2006</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>64</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>2530</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28" t="str">
-            <v>FY22</v>
-          </cell>
-          <cell r="D28">
-            <v>44911</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>3.0577866054115437</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>5.6247399954088877</v>
+            <v>2013</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>FY21</v>
+          </cell>
+          <cell r="D30">
+            <v>45195</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>1.7973947764799401</v>
+            <v>0.91229633789258391</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>2.2528786210358729</v>
+            <v>0.56696729484494968</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>9.2982580275560043</v>
+            <v>0.69130671053943571</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>3.9507486538127492</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="C39">
+            <v>4.8171721382664581</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="12">
-          <cell r="R12">
-            <v>18.783999999999999</v>
-          </cell>
-          <cell r="S12">
-            <v>22.285</v>
-          </cell>
-          <cell r="T12">
-            <v>1.3850000000000033</v>
-          </cell>
-          <cell r="U12">
-            <v>1.7280000000000051</v>
-          </cell>
-          <cell r="V12">
-            <v>37.451000000000015</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="V16">
-            <v>0.84829230777171583</v>
-          </cell>
-          <cell r="AO16">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="V17">
-            <v>0.28620168162650139</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="V18">
-            <v>0.19330446317506367</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="V19">
-            <v>0.19744990892531872</v>
-          </cell>
-        </row>
         <row r="20">
-          <cell r="AO20">
-            <v>9.417179548242931</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="M21">
-            <v>0.5227927414761171</v>
-          </cell>
-          <cell r="R21">
-            <v>5.7735504703074536E-2</v>
-          </cell>
-          <cell r="S21">
-            <v>7.7529282941235067E-2</v>
-          </cell>
-          <cell r="T21">
-            <v>-0.38817035428888169</v>
-          </cell>
-          <cell r="U21">
-            <v>-9.5567047928227233E-2</v>
-          </cell>
-          <cell r="V21">
-            <v>1.6954144522663404</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="AO22">
-            <v>2.9818941007369681</v>
+          <cell r="K20">
+            <v>2.2430000000000003</v>
+          </cell>
+          <cell r="L20">
+            <v>-9.4930000000000021</v>
+          </cell>
+          <cell r="M20">
+            <v>4.2279999999999998</v>
+          </cell>
+          <cell r="N20">
+            <v>5.7570000000000006</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="K24">
+            <v>1.073164572943619E-2</v>
+          </cell>
+          <cell r="L24">
+            <v>-0.29357941415277</v>
+          </cell>
+          <cell r="M24">
+            <v>-0.40139693205428584</v>
+          </cell>
+          <cell r="N24">
+            <v>1.9625581567092532</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="N27">
+            <v>0.86972778941070894</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="N28">
+            <v>0.21161132715126135</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="N29">
+            <v>0.14350882440921331</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="N30">
+            <v>0.21641486320947326</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1055,20 +1261,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9B459D-57D2-4CEE-BA00-1FA84E38A658}">
-  <dimension ref="B2:AV5"/>
+  <dimension ref="B2:AV14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AN3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U18" sqref="U18"/>
+      <selection pane="bottomRight" activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="9.140625" style="12"/>
     <col min="7" max="10" width="9.140625" style="9"/>
@@ -1223,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>[3]Main!$B$3</f>
+        <f>[1]Main!$B$3</f>
         <v>Hollywood Bowl Group Plc</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1233,143 +1439,143 @@
         <v>42</v>
       </c>
       <c r="F3" s="12">
-        <f>[3]Main!$C$6</f>
+        <f>[1]Main!$C$6</f>
         <v>2.3650000000000002</v>
       </c>
       <c r="G3" s="9">
-        <f>[3]Main!$C$7</f>
+        <f>[1]Main!$C$7</f>
         <v>170.949286</v>
       </c>
       <c r="H3" s="9">
-        <f>[3]Main!$C$8</f>
+        <f>[1]Main!$C$8</f>
         <v>404.29506139000006</v>
       </c>
       <c r="I3" s="9">
-        <f>[3]Main!$C$11</f>
+        <f>[1]Main!$C$11</f>
         <v>56.066000000000003</v>
       </c>
       <c r="J3" s="9">
-        <f>[3]Main!$C$12</f>
+        <f>[1]Main!$C$12</f>
         <v>348.22906139000008</v>
       </c>
       <c r="K3" s="2" t="str">
-        <f>[3]Main!$C$28</f>
+        <f>[1]Main!$C$28</f>
         <v>FY22</v>
       </c>
       <c r="L3" s="15">
-        <f>[3]Main!$D$28</f>
+        <f>[1]Main!$D$28</f>
         <v>44911</v>
       </c>
       <c r="M3" s="19">
-        <f>'[3]Financial Model'!$AO$20</f>
+        <f>'[1]Financial Model'!$AO$20</f>
         <v>9.417179548242931</v>
       </c>
       <c r="N3" s="20">
-        <f>'[3]Financial Model'!$AO$22</f>
+        <f>'[1]Financial Model'!$AO$22</f>
         <v>2.9818941007369681</v>
       </c>
       <c r="O3" s="20">
-        <f>'[3]Financial Model'!$AO$16</f>
+        <f>'[1]Financial Model'!$AO$16</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q3" s="10">
-        <f>[3]Main!$C$33</f>
+        <f>[1]Main!$C$33</f>
         <v>3.0577866054115437</v>
       </c>
       <c r="R3" s="10">
-        <f>[3]Main!$C$34</f>
+        <f>[1]Main!$C$34</f>
         <v>5.6247399954088877</v>
       </c>
       <c r="S3" s="10">
-        <f>[3]Main!$C$35</f>
+        <f>[1]Main!$C$35</f>
         <v>1.7973947764799401</v>
       </c>
       <c r="T3" s="10">
-        <f>[3]Main!$C$36</f>
+        <f>[1]Main!$C$36</f>
         <v>2.2528786210358729</v>
       </c>
       <c r="U3" s="10">
-        <f>[3]Main!$C$37</f>
+        <f>[1]Main!$C$37</f>
         <v>9.2982580275560043</v>
       </c>
       <c r="W3" s="14">
-        <f>'[3]Financial Model'!$V$12</f>
+        <f>'[1]Financial Model'!$V$12</f>
         <v>37.451000000000015</v>
       </c>
       <c r="X3" s="14">
-        <f>'[3]Financial Model'!$U$12</f>
+        <f>'[1]Financial Model'!$U$12</f>
         <v>1.7280000000000051</v>
       </c>
       <c r="Y3" s="14">
-        <f>'[3]Financial Model'!$T$12</f>
+        <f>'[1]Financial Model'!$T$12</f>
         <v>1.3850000000000033</v>
       </c>
       <c r="Z3" s="14">
-        <f>'[3]Financial Model'!$S$12</f>
+        <f>'[1]Financial Model'!$S$12</f>
         <v>22.285</v>
       </c>
       <c r="AA3" s="14">
-        <f>'[3]Financial Model'!$R$12</f>
+        <f>'[1]Financial Model'!$R$12</f>
         <v>18.783999999999999</v>
       </c>
       <c r="AC3" s="16">
-        <f>'[3]Financial Model'!$V$16</f>
+        <f>'[1]Financial Model'!$V$16</f>
         <v>0.84829230777171583</v>
       </c>
       <c r="AD3" s="16">
-        <f>'[3]Financial Model'!$V$17</f>
+        <f>'[1]Financial Model'!$V$17</f>
         <v>0.28620168162650139</v>
       </c>
       <c r="AE3" s="16">
-        <f>'[3]Financial Model'!$V$18</f>
+        <f>'[1]Financial Model'!$V$18</f>
         <v>0.19330446317506367</v>
       </c>
       <c r="AF3" s="16">
-        <f>'[3]Financial Model'!$V$19</f>
+        <f>'[1]Financial Model'!$V$19</f>
         <v>0.19744990892531872</v>
       </c>
       <c r="AH3" s="16">
-        <f>'[3]Financial Model'!$M$21</f>
+        <f>'[1]Financial Model'!$M$21</f>
         <v>0.5227927414761171</v>
       </c>
       <c r="AI3" s="16">
-        <f>'[3]Financial Model'!$V$21</f>
+        <f>'[1]Financial Model'!$V$21</f>
         <v>1.6954144522663404</v>
       </c>
       <c r="AJ3" s="16">
-        <f>'[3]Financial Model'!$U$21</f>
+        <f>'[1]Financial Model'!$U$21</f>
         <v>-9.5567047928227233E-2</v>
       </c>
       <c r="AK3" s="16">
-        <f>'[3]Financial Model'!$T$21</f>
+        <f>'[1]Financial Model'!$T$21</f>
         <v>-0.38817035428888169</v>
       </c>
       <c r="AL3" s="16">
-        <f>'[3]Financial Model'!$S$21</f>
+        <f>'[1]Financial Model'!$S$21</f>
         <v>7.7529282941235067E-2</v>
       </c>
       <c r="AM3" s="16">
-        <f>'[3]Financial Model'!$R$21</f>
+        <f>'[1]Financial Model'!$R$21</f>
         <v>5.7735504703074536E-2</v>
       </c>
       <c r="AO3" s="17">
-        <f>[3]Main!$C$25</f>
+        <f>[1]Main!$C$25</f>
         <v>64</v>
       </c>
       <c r="AP3" s="17">
-        <f>[3]Main!$C$26</f>
+        <f>[1]Main!$C$26</f>
         <v>2530</v>
       </c>
       <c r="AQ3" s="2">
-        <f>[3]Main!$C$24</f>
+        <f>[1]Main!$C$24</f>
         <v>2010</v>
       </c>
       <c r="AR3" s="2">
-        <f>[3]Main!$C$27</f>
+        <f>[1]Main!$C$27</f>
         <v>2016</v>
       </c>
       <c r="AS3" s="2" t="str">
-        <f>[3]Main!$C$23</f>
+        <f>[1]Main!$C$23</f>
         <v>Hemel, UK</v>
       </c>
       <c r="AU3" s="2" t="s">
@@ -1384,7 +1590,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>[1]Main!$B$3</f>
+        <f>[2]Main!$B$3</f>
         <v>Ten Entertainment Group Plc</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1394,123 +1600,123 @@
         <v>42</v>
       </c>
       <c r="F4" s="12">
-        <f>[1]Main!$C$6</f>
+        <f>[2]Main!$C$6</f>
         <v>2.7210000000000001</v>
       </c>
       <c r="G4" s="9">
-        <f>[1]Main!$C$7</f>
+        <f>[2]Main!$C$7</f>
         <v>68.381495999999999</v>
       </c>
       <c r="H4" s="9">
-        <f>[1]Main!$C$8</f>
+        <f>[2]Main!$C$8</f>
         <v>186.06605061600001</v>
       </c>
       <c r="I4" s="9">
-        <f>[1]Main!$C$11</f>
+        <f>[2]Main!$C$11</f>
         <v>-200.21699999999998</v>
       </c>
       <c r="J4" s="9">
-        <f>[1]Main!$C$12</f>
+        <f>[2]Main!$C$12</f>
         <v>386.28305061599997</v>
       </c>
       <c r="K4" s="2" t="str">
-        <f>[1]Main!$C$28</f>
+        <f>[2]Main!$C$28</f>
         <v>H122</v>
       </c>
       <c r="L4" s="15">
-        <f>[1]Main!$D$28</f>
+        <f>[2]Main!$D$28</f>
         <v>45190</v>
       </c>
       <c r="Q4" s="10">
-        <f>[1]Main!$C$33</f>
+        <f>[2]Main!$C$33</f>
         <v>3.5367722369936718</v>
       </c>
       <c r="R4" s="10">
-        <f>[1]Main!$C$34</f>
+        <f>[2]Main!$C$34</f>
         <v>1.5486275426012701</v>
       </c>
       <c r="S4" s="10">
-        <f>[1]Main!$C$35</f>
+        <f>[2]Main!$C$35</f>
         <v>3.215033421967723</v>
       </c>
       <c r="T4" s="10">
-        <f>[1]Main!$C$36</f>
+        <f>[2]Main!$C$36</f>
         <v>5.9823787638134727</v>
       </c>
       <c r="U4" s="10">
-        <f>[1]Main!$C$37</f>
+        <f>[2]Main!$C$37</f>
         <v>12.421475677406907</v>
       </c>
       <c r="X4" s="14">
-        <f>'[1]Financial Model'!$S$19</f>
+        <f>'[2]Financial Model'!$S$19</f>
         <v>4.005000000000007</v>
       </c>
       <c r="Y4" s="14">
-        <f>'[1]Financial Model'!$R$19</f>
+        <f>'[2]Financial Model'!$R$19</f>
         <v>-17.747</v>
       </c>
       <c r="Z4" s="14">
-        <f>'[1]Financial Model'!$Q$19</f>
+        <f>'[2]Financial Model'!$Q$19</f>
         <v>9.036999999999999</v>
       </c>
       <c r="AA4" s="14">
-        <f>'[1]Financial Model'!$P$19</f>
+        <f>'[2]Financial Model'!$P$19</f>
         <v>8.1420000000000101</v>
       </c>
       <c r="AC4" s="16">
-        <f>'[1]Financial Model'!$K$26</f>
+        <f>'[2]Financial Model'!$K$26</f>
         <v>0.68836775356589386</v>
       </c>
       <c r="AD4" s="16">
-        <f>'[1]Financial Model'!$K$27</f>
+        <f>'[2]Financial Model'!$K$27</f>
         <v>0.38816850627787092</v>
       </c>
       <c r="AE4" s="16">
-        <f>'[1]Financial Model'!$K$28</f>
+        <f>'[2]Financial Model'!$K$28</f>
         <v>0.2892880862772384</v>
       </c>
       <c r="AF4" s="16">
-        <f>'[1]Financial Model'!$K$29</f>
+        <f>'[2]Financial Model'!$K$29</f>
         <v>5.0590924103622523E-3</v>
       </c>
       <c r="AH4" s="16">
-        <f>'[1]Financial Model'!$K$23</f>
+        <f>'[2]Financial Model'!$K$23</f>
         <v>4.9602262016965133</v>
       </c>
       <c r="AJ4" s="16">
-        <f>'[1]Financial Model'!$S$23</f>
+        <f>'[2]Financial Model'!$S$23</f>
         <v>0.86167250268824636</v>
       </c>
       <c r="AK4" s="16">
-        <f>'[1]Financial Model'!$R$23</f>
+        <f>'[2]Financial Model'!$R$23</f>
         <v>-0.56885238106559521</v>
       </c>
       <c r="AL4" s="16">
-        <f>'[1]Financial Model'!$Q$23</f>
+        <f>'[2]Financial Model'!$Q$23</f>
         <v>0.10179436804191222</v>
       </c>
       <c r="AM4" s="16">
-        <f>'[1]Financial Model'!$P$23</f>
+        <f>'[2]Financial Model'!$P$23</f>
         <v>7.4746621621621712E-2</v>
       </c>
       <c r="AO4" s="17">
-        <f>[1]Main!$C$25</f>
+        <f>[2]Main!$C$25</f>
         <v>48</v>
       </c>
       <c r="AP4" s="17">
-        <f>[1]Main!$C$26</f>
+        <f>[2]Main!$C$26</f>
         <v>1500</v>
       </c>
       <c r="AQ4" s="2">
-        <f>[1]Main!$C$24</f>
+        <f>[2]Main!$C$24</f>
         <v>2009</v>
       </c>
       <c r="AR4" s="18">
-        <f>[1]Main!$C$27</f>
+        <f>[2]Main!$C$27</f>
         <v>2017</v>
       </c>
       <c r="AS4" s="2" t="str">
-        <f>[1]Main!$C$23</f>
+        <f>[2]Main!$C$23</f>
         <v>Cranfield, UK</v>
       </c>
       <c r="AU4" s="2" t="s">
@@ -1525,7 +1731,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>[2]Main!$B$3</f>
+        <f>[3]Main!$B$3</f>
         <v>Cineworld Group Plc.</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1535,43 +1741,43 @@
         <v>42</v>
       </c>
       <c r="F5" s="12">
-        <f>[2]Main!$C$6</f>
+        <f>[3]Main!$C$6</f>
         <v>2.7E-2</v>
       </c>
       <c r="G5" s="9">
-        <f>[2]Main!$C$7</f>
+        <f>[3]Main!$C$7</f>
         <v>1370</v>
       </c>
       <c r="H5" s="9">
-        <f>[2]Main!$C$8</f>
+        <f>[3]Main!$C$8</f>
         <v>36.99</v>
       </c>
       <c r="I5" s="9">
-        <f>[2]Main!$C$11</f>
+        <f>[3]Main!$C$11</f>
         <v>-4013.2990000000004</v>
       </c>
       <c r="J5" s="9">
-        <f>[2]Main!$C$12</f>
+        <f>[3]Main!$C$12</f>
         <v>4050.2890000000002</v>
       </c>
       <c r="K5" s="22" t="str">
-        <f>[2]Main!$C$27</f>
+        <f>[3]Main!$C$27</f>
         <v>FY21</v>
       </c>
       <c r="L5" s="23">
-        <f>[2]Main!$D$27</f>
+        <f>[3]Main!$D$27</f>
         <v>44287</v>
       </c>
       <c r="AO5" s="17">
-        <f>[2]Main!$C$26</f>
+        <f>[3]Main!$C$26</f>
         <v>751</v>
       </c>
       <c r="AQ5" s="2">
-        <f>[2]Main!$C$24</f>
+        <f>[3]Main!$C$24</f>
         <v>1995</v>
       </c>
       <c r="AS5" s="2" t="str">
-        <f>[2]Main!$C$23</f>
+        <f>[3]Main!$C$23</f>
         <v>Brentford, UK</v>
       </c>
       <c r="AU5" s="2" t="s">
@@ -1579,6 +1785,226 @@
       </c>
       <c r="AV5" s="2" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="12">
+        <f>[4]Main!$C$6</f>
+        <v>0.61</v>
+      </c>
+      <c r="G6" s="9">
+        <f>[4]Main!$C$7</f>
+        <v>37.286000000000001</v>
+      </c>
+      <c r="H6" s="9">
+        <f>[4]Main!$C$8</f>
+        <v>22.74446</v>
+      </c>
+      <c r="I6" s="9">
+        <f>[4]Main!$C$11</f>
+        <v>-4.9880000000000013</v>
+      </c>
+      <c r="J6" s="9">
+        <f>[4]Main!$C$12</f>
+        <v>27.732460000000003</v>
+      </c>
+      <c r="K6" s="31" t="str">
+        <f>[4]Main!$C$30</f>
+        <v>FY21</v>
+      </c>
+      <c r="L6" s="15">
+        <f>[4]Main!$D$30</f>
+        <v>45195</v>
+      </c>
+      <c r="Q6" s="10">
+        <f>[4]Main!$C$35</f>
+        <v>0.91229633789258391</v>
+      </c>
+      <c r="R6" s="10">
+        <f>[4]Main!$C$36</f>
+        <v>0.56696729484494968</v>
+      </c>
+      <c r="S6" s="10">
+        <f>[4]Main!$C$37</f>
+        <v>0.69130671053943571</v>
+      </c>
+      <c r="T6" s="10">
+        <f>[4]Main!$C$38</f>
+        <v>3.9507486538127492</v>
+      </c>
+      <c r="U6" s="10">
+        <f>[4]Main!$C$39</f>
+        <v>4.8171721382664581</v>
+      </c>
+      <c r="X6" s="14">
+        <f>'[4]Financial Model'!$N$20</f>
+        <v>5.7570000000000006</v>
+      </c>
+      <c r="Y6" s="14">
+        <f>'[4]Financial Model'!$M$20</f>
+        <v>4.2279999999999998</v>
+      </c>
+      <c r="Z6" s="14">
+        <f>'[4]Financial Model'!$L$20</f>
+        <v>-9.4930000000000021</v>
+      </c>
+      <c r="AA6" s="14">
+        <f>'[4]Financial Model'!$K$20</f>
+        <v>2.2430000000000003</v>
+      </c>
+      <c r="AC6" s="16">
+        <f>'[4]Financial Model'!$N$27</f>
+        <v>0.86972778941070894</v>
+      </c>
+      <c r="AD6" s="16">
+        <f>'[4]Financial Model'!$N$28</f>
+        <v>0.21161132715126135</v>
+      </c>
+      <c r="AE6" s="16">
+        <f>'[4]Financial Model'!$N$29</f>
+        <v>0.14350882440921331</v>
+      </c>
+      <c r="AF6" s="16">
+        <f>'[4]Financial Model'!$N$30</f>
+        <v>0.21641486320947326</v>
+      </c>
+      <c r="AJ6" s="16">
+        <f>'[4]Financial Model'!$N$24</f>
+        <v>1.9625581567092532</v>
+      </c>
+      <c r="AK6" s="16">
+        <f>'[4]Financial Model'!$M$24</f>
+        <v>-0.40139693205428584</v>
+      </c>
+      <c r="AL6" s="16">
+        <f>'[4]Financial Model'!$L$24</f>
+        <v>-0.29357941415277</v>
+      </c>
+      <c r="AM6" s="16">
+        <f>'[4]Financial Model'!$K$24</f>
+        <v>1.073164572943619E-2</v>
+      </c>
+      <c r="AQ6" s="2">
+        <f>[4]Main!$C$24</f>
+        <v>2006</v>
+      </c>
+      <c r="AR6" s="2">
+        <f>[4]Main!$C$25</f>
+        <v>2013</v>
+      </c>
+      <c r="AS6" s="2" t="str">
+        <f>[4]Main!$C$23</f>
+        <v>London, UK</v>
+      </c>
+      <c r="AU6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="11" spans="2:48" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29"/>
+      <c r="AC11" s="25"/>
+      <c r="AD11" s="25"/>
+      <c r="AE11" s="25"/>
+      <c r="AF11" s="25"/>
+      <c r="AH11" s="25"/>
+      <c r="AI11" s="25"/>
+      <c r="AJ11" s="25"/>
+      <c r="AK11" s="25"/>
+      <c r="AL11" s="25"/>
+      <c r="AM11" s="25"/>
+      <c r="AO11" s="30"/>
+      <c r="AP11" s="30"/>
+      <c r="AQ11" s="25"/>
+      <c r="AR11" s="25"/>
+      <c r="AS11" s="25"/>
+      <c r="AU11" s="25"/>
+      <c r="AV11" s="25"/>
+    </row>
+    <row r="12" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:48" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1586,7 +2012,9 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{54EAB678-1952-4221-81BE-1A742E0604C2}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{C8996EB5-A490-40A7-9AEE-007EA928F60C}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{116C4D30-3ED6-47C4-92C7-1DCF584CA6FB}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{AC06FEE0-38B8-4446-93BB-C1421D99C291}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$RBLX Q2, £MHC H1 update (half finished)
</commit_message>
<xml_diff>
--- a/Overview - Leisure Facilities.xlsx
+++ b/Overview - Leisure Facilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83027669-7A60-4C10-BF9E-2127AD998496}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BE4506-0B32-42F5-9E92-3009446BC0D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5EB38F2A-A5E5-4604-9A50-AFDB2AF73DAE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="76">
   <si>
     <t>Ticker</t>
   </si>
@@ -470,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -575,6 +575,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1658,7 +1664,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1848,11 +1854,11 @@
         <f>[1]Main!$C$12*G29</f>
         <v>2865.8142033854997</v>
       </c>
-      <c r="K3" s="2" t="str">
+      <c r="K3" s="22" t="str">
         <f>[1]Main!$C$30</f>
         <v>Q223</v>
       </c>
-      <c r="L3" s="33">
+      <c r="L3" s="23">
         <f>[1]Main!$D$30</f>
         <v>44958</v>
       </c>
@@ -2098,11 +2104,11 @@
         <f>[4]Main!$C$12</f>
         <v>386.28305061599997</v>
       </c>
-      <c r="K5" s="2" t="str">
+      <c r="K5" s="22" t="str">
         <f>[4]Main!$C$28</f>
         <v>H122</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="41">
         <f>[4]Main!$D$28</f>
         <v>45190</v>
       </c>
@@ -2387,11 +2393,11 @@
         <f>[7]Main!$C$12</f>
         <v>27.732460000000003</v>
       </c>
-      <c r="K8" s="31" t="str">
+      <c r="K8" s="40" t="str">
         <f>[7]Main!$C$30</f>
         <v>FY21</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="41">
         <f>[7]Main!$D$30</f>
         <v>45195</v>
       </c>

</xml_diff>

<commit_message>
£TEG FY22 results, update overview
</commit_message>
<xml_diff>
--- a/Overview - Leisure Facilities.xlsx
+++ b/Overview - Leisure Facilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06681B6-4935-4EFF-AD75-8503DE3D1232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2CF5F6-D5AC-4880-8F2B-01D13868A01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5EB38F2A-A5E5-4604-9A50-AFDB2AF73DAE}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>Ticker</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>24/7 No Contract Fitness Clubs</t>
+  </si>
+  <si>
+    <t>FY23 E</t>
   </si>
 </sst>
 </file>
@@ -967,12 +970,7 @@
         </row>
         <row r="25">
           <cell r="C25">
-            <v>48</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>1500</v>
+            <v>51</v>
           </cell>
         </row>
         <row r="27">
@@ -995,22 +993,22 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>1.5677560737084784</v>
+            <v>1.4632398140308083</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>3.2471957694196369</v>
+            <v>3.0307177331023607</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>6.046138037665215</v>
+            <v>9.1425678056593718</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>12.545736848028811</v>
+            <v>18.93643277678008</v>
           </cell>
         </row>
       </sheetData>
@@ -1028,6 +1026,9 @@
           <cell r="U19">
             <v>4.005000000000007</v>
           </cell>
+          <cell r="V19">
+            <v>26.596000000000004</v>
+          </cell>
         </row>
         <row r="23">
           <cell r="M23">
@@ -1045,6 +1046,9 @@
           <cell r="U23">
             <v>0.86167250268824636</v>
           </cell>
+          <cell r="V23">
+            <v>0.87605337598673017</v>
+          </cell>
         </row>
         <row r="26">
           <cell r="M26">
@@ -1064,6 +1068,11 @@
         <row r="29">
           <cell r="M29">
             <v>3.4631110778390712E-3</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="V38">
+            <v>1673</v>
           </cell>
         </row>
       </sheetData>
@@ -1679,13 +1688,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9B459D-57D2-4CEE-BA00-1FA84E38A658}">
-  <dimension ref="B2:AV29"/>
+  <dimension ref="B2:AW29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH6" sqref="AH6"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1700,24 +1709,24 @@
     <col min="13" max="15" width="9.140625" style="6"/>
     <col min="16" max="16" width="9.140625" style="1"/>
     <col min="17" max="21" width="9.140625" style="2"/>
-    <col min="22" max="22" width="9.140625" style="1"/>
-    <col min="23" max="27" width="9.140625" style="14"/>
-    <col min="28" max="28" width="9.140625" style="1"/>
-    <col min="29" max="32" width="9.140625" style="2"/>
-    <col min="33" max="33" width="9.140625" style="1"/>
-    <col min="34" max="39" width="9.140625" style="2"/>
-    <col min="40" max="40" width="9.140625" style="1"/>
-    <col min="41" max="41" width="9.140625" style="17"/>
-    <col min="42" max="42" width="10.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="9.140625" style="2"/>
-    <col min="45" max="45" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="1"/>
-    <col min="47" max="47" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="45.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="1"/>
+    <col min="22" max="23" width="9.140625" style="1"/>
+    <col min="24" max="28" width="9.140625" style="14"/>
+    <col min="29" max="29" width="9.140625" style="1"/>
+    <col min="30" max="33" width="9.140625" style="2"/>
+    <col min="34" max="34" width="9.140625" style="1"/>
+    <col min="35" max="40" width="9.140625" style="2"/>
+    <col min="41" max="41" width="9.140625" style="1"/>
+    <col min="42" max="42" width="9.140625" style="17"/>
+    <col min="43" max="43" width="10.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="9.140625" style="2"/>
+    <col min="46" max="46" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.140625" style="1"/>
+    <col min="48" max="48" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="45.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:48" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1775,74 +1784,77 @@
       <c r="U2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="Y2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Z2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="AA2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AB2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AO2" s="21" t="s">
+      <c r="AP2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AP2" s="21" t="s">
+      <c r="AQ2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>67</v>
       </c>
@@ -1887,50 +1899,50 @@
         <f>[1]Main!$C$35</f>
         <v>16.995954373839119</v>
       </c>
-      <c r="AC3" s="16">
+      <c r="AD3" s="16">
         <f>'[1]Financial Models'!$L$30</f>
         <v>0.34266327706348176</v>
       </c>
-      <c r="AD3" s="16">
+      <c r="AE3" s="16">
         <f>'[1]Financial Models'!$L$31</f>
         <v>0.22106553029610243</v>
       </c>
-      <c r="AE3" s="16">
+      <c r="AF3" s="16">
         <f>'[1]Financial Models'!$L$32</f>
         <v>5.2490078094992289E-3</v>
       </c>
-      <c r="AF3" s="16">
+      <c r="AG3" s="16">
         <f>'[1]Financial Models'!$L$33</f>
         <v>0.51503886448125302</v>
       </c>
-      <c r="AH3" s="16">
+      <c r="AI3" s="16">
         <f>'[1]Financial Models'!$L$27</f>
         <v>0.46816180042942013</v>
       </c>
-      <c r="AO3" s="17">
+      <c r="AP3" s="17">
         <f>[1]Main!$C$28</f>
         <v>327</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="AR3" s="2">
         <f>[1]Main!$C$24</f>
         <v>1997</v>
       </c>
-      <c r="AR3" s="2">
+      <c r="AS3" s="2">
         <f>[1]Main!$C$25</f>
         <v>2021</v>
       </c>
-      <c r="AS3" s="2" t="str">
+      <c r="AT3" s="2" t="str">
         <f>[1]Main!$C$23</f>
         <v>Mechanicsville, VA</v>
       </c>
-      <c r="AU3" s="2" t="s">
+      <c r="AV3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AW3" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2004,94 +2016,94 @@
         <f>[3]Main!$C$37</f>
         <v>9.2982580275560043</v>
       </c>
-      <c r="W4" s="14">
+      <c r="X4" s="14">
         <f>'[3]Financial Model'!$V$12</f>
         <v>37.451000000000015</v>
       </c>
-      <c r="X4" s="14">
+      <c r="Y4" s="14">
         <f>'[3]Financial Model'!$U$12</f>
         <v>1.7280000000000051</v>
       </c>
-      <c r="Y4" s="14">
+      <c r="Z4" s="14">
         <f>'[3]Financial Model'!$T$12</f>
         <v>1.3850000000000033</v>
       </c>
-      <c r="Z4" s="14">
+      <c r="AA4" s="14">
         <f>'[3]Financial Model'!$S$12</f>
         <v>22.285</v>
       </c>
-      <c r="AA4" s="14">
+      <c r="AB4" s="14">
         <f>'[3]Financial Model'!$R$12</f>
         <v>18.783999999999999</v>
       </c>
-      <c r="AC4" s="16">
+      <c r="AD4" s="16">
         <f>'[3]Financial Model'!$V$16</f>
         <v>0.84829230777171583</v>
       </c>
-      <c r="AD4" s="16">
+      <c r="AE4" s="16">
         <f>'[3]Financial Model'!$V$17</f>
         <v>0.28620168162650139</v>
       </c>
-      <c r="AE4" s="16">
+      <c r="AF4" s="16">
         <f>'[3]Financial Model'!$V$18</f>
         <v>0.19330446317506367</v>
       </c>
-      <c r="AF4" s="16">
+      <c r="AG4" s="16">
         <f>'[3]Financial Model'!$V$19</f>
         <v>0.19744990892531872</v>
       </c>
-      <c r="AH4" s="16">
+      <c r="AI4" s="16">
         <f>'[3]Financial Model'!$M$21</f>
         <v>0.5227927414761171</v>
       </c>
-      <c r="AI4" s="16">
+      <c r="AJ4" s="16">
         <f>'[3]Financial Model'!$V$21</f>
         <v>1.6954144522663404</v>
       </c>
-      <c r="AJ4" s="16">
+      <c r="AK4" s="16">
         <f>'[3]Financial Model'!$U$21</f>
         <v>-9.5567047928227233E-2</v>
       </c>
-      <c r="AK4" s="16">
+      <c r="AL4" s="16">
         <f>'[3]Financial Model'!$T$21</f>
         <v>-0.38817035428888169</v>
       </c>
-      <c r="AL4" s="16">
+      <c r="AM4" s="16">
         <f>'[3]Financial Model'!$S$21</f>
         <v>7.7529282941235067E-2</v>
       </c>
-      <c r="AM4" s="16">
+      <c r="AN4" s="16">
         <f>'[3]Financial Model'!$R$21</f>
         <v>5.7735504703074536E-2</v>
       </c>
-      <c r="AO4" s="17">
+      <c r="AP4" s="17">
         <f>[3]Main!$C$25</f>
         <v>64</v>
       </c>
-      <c r="AP4" s="17">
+      <c r="AQ4" s="17">
         <f>[3]Main!$C$26</f>
         <v>2530</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AR4" s="2">
         <f>[3]Main!$C$24</f>
         <v>2010</v>
       </c>
-      <c r="AR4" s="2">
+      <c r="AS4" s="2">
         <f>[3]Main!$C$27</f>
         <v>2016</v>
       </c>
-      <c r="AS4" s="2" t="str">
+      <c r="AT4" s="2" t="str">
         <f>[3]Main!$C$23</f>
         <v>Hemel, UK</v>
       </c>
-      <c r="AU4" s="2" t="s">
+      <c r="AV4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV4" s="2" t="s">
+      <c r="AW4" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2139,100 +2151,108 @@
       </c>
       <c r="R5" s="10">
         <f>[4]Main!$C$34</f>
-        <v>1.5677560737084784</v>
+        <v>1.4632398140308083</v>
       </c>
       <c r="S5" s="10">
         <f>[4]Main!$C$35</f>
-        <v>3.2471957694196369</v>
+        <v>3.0307177331023607</v>
       </c>
       <c r="T5" s="10">
         <f>[4]Main!$C$36</f>
-        <v>6.046138037665215</v>
+        <v>9.1425678056593718</v>
       </c>
       <c r="U5" s="10">
         <f>[4]Main!$C$37</f>
-        <v>12.545736848028811</v>
+        <v>18.93643277678008</v>
       </c>
       <c r="X5" s="14">
+        <f>'[4]Financial Model'!$V$19</f>
+        <v>26.596000000000004</v>
+      </c>
+      <c r="Y5" s="14">
         <f>'[4]Financial Model'!$U$19</f>
         <v>4.005000000000007</v>
       </c>
-      <c r="Y5" s="14">
+      <c r="Z5" s="14">
         <f>'[4]Financial Model'!$T$19</f>
         <v>-17.747</v>
       </c>
-      <c r="Z5" s="14">
+      <c r="AA5" s="14">
         <f>'[4]Financial Model'!$S$19</f>
         <v>9.036999999999999</v>
       </c>
-      <c r="AA5" s="14">
+      <c r="AB5" s="14">
         <f>'[4]Financial Model'!$R$19</f>
         <v>8.1420000000000101</v>
       </c>
-      <c r="AC5" s="16">
+      <c r="AD5" s="16">
         <f>'[4]Financial Model'!$M$26</f>
         <v>0.67520215633423175</v>
       </c>
-      <c r="AD5" s="16">
+      <c r="AE5" s="16">
         <f>'[4]Financial Model'!$M$27</f>
         <v>0.2960365106591521</v>
       </c>
-      <c r="AE5" s="16">
+      <c r="AF5" s="16">
         <f>'[4]Financial Model'!$M$28</f>
         <v>0.18838826268071546</v>
       </c>
-      <c r="AF5" s="16">
+      <c r="AG5" s="16">
         <f>'[4]Financial Model'!$M$29</f>
         <v>3.4631110778390712E-3</v>
       </c>
-      <c r="AH5" s="16">
+      <c r="AI5" s="16">
         <f>'[4]Financial Model'!$M$23</f>
         <v>3.254372371042713E-2</v>
       </c>
       <c r="AJ5" s="16">
+        <f>'[4]Financial Model'!$V$23</f>
+        <v>0.87605337598673017</v>
+      </c>
+      <c r="AK5" s="16">
         <f>'[4]Financial Model'!$U$23</f>
         <v>0.86167250268824636</v>
       </c>
-      <c r="AK5" s="16">
+      <c r="AL5" s="16">
         <f>'[4]Financial Model'!$T$23</f>
         <v>-0.56885238106559521</v>
       </c>
-      <c r="AL5" s="16">
+      <c r="AM5" s="16">
         <f>'[4]Financial Model'!$S$23</f>
         <v>0.10179436804191222</v>
       </c>
-      <c r="AM5" s="16">
+      <c r="AN5" s="16">
         <f>'[4]Financial Model'!$R$23</f>
         <v>7.4746621621621712E-2</v>
       </c>
-      <c r="AO5" s="17">
+      <c r="AP5" s="17">
         <f>[4]Main!$C$25</f>
-        <v>48</v>
-      </c>
-      <c r="AP5" s="17">
-        <f>[4]Main!$C$26</f>
-        <v>1500</v>
-      </c>
-      <c r="AQ5" s="2">
+        <v>51</v>
+      </c>
+      <c r="AQ5" s="17">
+        <f>'[4]Financial Model'!$V$38</f>
+        <v>1673</v>
+      </c>
+      <c r="AR5" s="2">
         <f>[4]Main!$C$24</f>
         <v>2009</v>
       </c>
-      <c r="AR5" s="18">
+      <c r="AS5" s="18">
         <f>[4]Main!$C$27</f>
         <v>2017</v>
       </c>
-      <c r="AS5" s="2" t="str">
+      <c r="AT5" s="2" t="str">
         <f>[4]Main!$C$23</f>
         <v>Cranfield, UK</v>
       </c>
-      <c r="AU5" s="2" t="s">
+      <c r="AV5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AV5" s="2" t="s">
+      <c r="AW5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>54</v>
       </c>
@@ -2285,42 +2305,42 @@
         <f>[5]Main!$C$37</f>
         <v>1.3656803323285136</v>
       </c>
-      <c r="AC6" s="16">
+      <c r="AD6" s="16">
         <f>'[5]Financial Model'!$Y$18</f>
         <v>0.9884326200115674</v>
       </c>
-      <c r="AI6" s="16">
+      <c r="AJ6" s="16">
         <f>'[5]Financial Model'!$Y$23</f>
         <v>0.63113207547169825</v>
       </c>
-      <c r="AO6" s="17">
+      <c r="AP6" s="17">
         <f>[5]Main!$C$28</f>
         <v>229</v>
       </c>
-      <c r="AP6" s="17">
+      <c r="AQ6" s="17">
         <f>[5]Main!$C$27</f>
         <v>0</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AR6" s="2">
         <f>[5]Main!$C$24</f>
         <v>2007</v>
       </c>
-      <c r="AR6" s="2">
+      <c r="AS6" s="2">
         <f>[5]Main!$C$25</f>
         <v>2015</v>
       </c>
-      <c r="AS6" s="2" t="str">
+      <c r="AT6" s="2" t="str">
         <f>[5]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AU6" s="2" t="s">
+      <c r="AV6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AV6" s="2" t="s">
+      <c r="AW6" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
@@ -2362,26 +2382,26 @@
         <f>[6]Main!$D$27</f>
         <v>44287</v>
       </c>
-      <c r="AO7" s="17">
+      <c r="AP7" s="17">
         <f>[6]Main!$C$26</f>
         <v>751</v>
       </c>
-      <c r="AQ7" s="2">
+      <c r="AR7" s="2">
         <f>[6]Main!$C$24</f>
         <v>1995</v>
       </c>
-      <c r="AS7" s="2" t="str">
+      <c r="AT7" s="2" t="str">
         <f>[6]Main!$C$23</f>
         <v>Brentford, UK</v>
       </c>
-      <c r="AU7" s="2" t="s">
+      <c r="AV7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AW7" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>60</v>
       </c>
@@ -2442,78 +2462,78 @@
         <f>[7]Main!$C$39</f>
         <v>4.8171721382664581</v>
       </c>
-      <c r="X8" s="14">
+      <c r="Y8" s="14">
         <f>'[7]Financial Model'!$N$20</f>
         <v>5.7570000000000006</v>
       </c>
-      <c r="Y8" s="14">
+      <c r="Z8" s="14">
         <f>'[7]Financial Model'!$M$20</f>
         <v>4.2279999999999998</v>
       </c>
-      <c r="Z8" s="14">
+      <c r="AA8" s="14">
         <f>'[7]Financial Model'!$L$20</f>
         <v>-9.4930000000000021</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AB8" s="14">
         <f>'[7]Financial Model'!$K$20</f>
         <v>2.2430000000000003</v>
       </c>
-      <c r="AC8" s="16">
+      <c r="AD8" s="16">
         <f>'[7]Financial Model'!$N$27</f>
         <v>0.86972778941070894</v>
       </c>
-      <c r="AD8" s="16">
+      <c r="AE8" s="16">
         <f>'[7]Financial Model'!$N$28</f>
         <v>0.21161132715126135</v>
       </c>
-      <c r="AE8" s="16">
+      <c r="AF8" s="16">
         <f>'[7]Financial Model'!$N$29</f>
         <v>0.14350882440921331</v>
       </c>
-      <c r="AF8" s="16">
+      <c r="AG8" s="16">
         <f>'[7]Financial Model'!$N$30</f>
         <v>0.21641486320947326</v>
       </c>
-      <c r="AJ8" s="16">
+      <c r="AK8" s="16">
         <f>'[7]Financial Model'!$N$24</f>
         <v>1.9625581567092532</v>
       </c>
-      <c r="AK8" s="16">
+      <c r="AL8" s="16">
         <f>'[7]Financial Model'!$M$24</f>
         <v>-0.40139693205428584</v>
       </c>
-      <c r="AL8" s="16">
+      <c r="AM8" s="16">
         <f>'[7]Financial Model'!$L$24</f>
         <v>-0.29357941415277</v>
       </c>
-      <c r="AM8" s="16">
+      <c r="AN8" s="16">
         <f>'[7]Financial Model'!$K$24</f>
         <v>1.073164572943619E-2</v>
       </c>
-      <c r="AO8" s="17">
+      <c r="AP8" s="17">
         <f>[7]Main!$C$28</f>
         <v>18</v>
       </c>
-      <c r="AQ8" s="2">
+      <c r="AR8" s="2">
         <f>[7]Main!$C$24</f>
         <v>2006</v>
       </c>
-      <c r="AR8" s="2">
+      <c r="AS8" s="2">
         <f>[7]Main!$C$25</f>
         <v>2013</v>
       </c>
-      <c r="AS8" s="2" t="str">
+      <c r="AT8" s="2" t="str">
         <f>[7]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AU8" s="2" t="s">
+      <c r="AV8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AV8" s="2" t="s">
+      <c r="AW8" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
       <c r="K9" s="31"/>
       <c r="L9" s="15"/>
@@ -2522,16 +2542,16 @@
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
-      <c r="AC9" s="16"/>
       <c r="AD9" s="16"/>
       <c r="AE9" s="16"/>
       <c r="AF9" s="16"/>
-      <c r="AJ9" s="16"/>
+      <c r="AG9" s="16"/>
       <c r="AK9" s="16"/>
       <c r="AL9" s="16"/>
       <c r="AM9" s="16"/>
+      <c r="AN9" s="16"/>
     </row>
-    <row r="10" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="K10" s="31"/>
       <c r="L10" s="15"/>
@@ -2540,16 +2560,16 @@
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
-      <c r="AC10" s="16"/>
       <c r="AD10" s="16"/>
       <c r="AE10" s="16"/>
       <c r="AF10" s="16"/>
-      <c r="AJ10" s="16"/>
+      <c r="AG10" s="16"/>
       <c r="AK10" s="16"/>
       <c r="AL10" s="16"/>
       <c r="AM10" s="16"/>
+      <c r="AN10" s="16"/>
     </row>
-    <row r="11" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
       <c r="K11" s="31"/>
       <c r="L11" s="15"/>
@@ -2558,16 +2578,16 @@
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
-      <c r="AC11" s="16"/>
       <c r="AD11" s="16"/>
       <c r="AE11" s="16"/>
       <c r="AF11" s="16"/>
-      <c r="AJ11" s="16"/>
+      <c r="AG11" s="16"/>
       <c r="AK11" s="16"/>
       <c r="AL11" s="16"/>
       <c r="AM11" s="16"/>
+      <c r="AN11" s="16"/>
     </row>
-    <row r="12" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="K12" s="31"/>
       <c r="L12" s="15"/>
@@ -2576,25 +2596,25 @@
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
-      <c r="AC12" s="16"/>
       <c r="AD12" s="16"/>
       <c r="AE12" s="16"/>
       <c r="AF12" s="16"/>
-      <c r="AJ12" s="16"/>
+      <c r="AG12" s="16"/>
       <c r="AK12" s="16"/>
       <c r="AL12" s="16"/>
       <c r="AM12" s="16"/>
+      <c r="AN12" s="16"/>
     </row>
-    <row r="13" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
     </row>
-    <row r="17" spans="2:48" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:49" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C17" s="34"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
@@ -2613,30 +2633,30 @@
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
-      <c r="W17" s="29"/>
       <c r="X17" s="29"/>
       <c r="Y17" s="29"/>
       <c r="Z17" s="29"/>
       <c r="AA17" s="29"/>
-      <c r="AC17" s="25"/>
+      <c r="AB17" s="29"/>
       <c r="AD17" s="25"/>
       <c r="AE17" s="25"/>
       <c r="AF17" s="25"/>
-      <c r="AH17" s="25"/>
+      <c r="AG17" s="25"/>
       <c r="AI17" s="25"/>
       <c r="AJ17" s="25"/>
       <c r="AK17" s="25"/>
       <c r="AL17" s="25"/>
       <c r="AM17" s="25"/>
-      <c r="AO17" s="30"/>
+      <c r="AN17" s="25"/>
       <c r="AP17" s="30"/>
-      <c r="AQ17" s="25"/>
+      <c r="AQ17" s="30"/>
       <c r="AR17" s="25"/>
       <c r="AS17" s="25"/>
-      <c r="AU17" s="25"/>
+      <c r="AT17" s="25"/>
       <c r="AV17" s="25"/>
+      <c r="AW17" s="25"/>
     </row>
-    <row r="18" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2661,7 +2681,7 @@
         <v>1735.2331919999999</v>
       </c>
     </row>
-    <row r="19" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
@@ -2686,7 +2706,7 @@
         <v>5293.1000700000004</v>
       </c>
     </row>
-    <row r="20" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:49" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
@@ -2711,7 +2731,7 @@
         <v>2326.3088939999998</v>
       </c>
     </row>
-    <row r="28" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:49" x14ac:dyDescent="0.2">
       <c r="F28" s="40" t="s">
         <v>71</v>
       </c>
@@ -2720,7 +2740,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:48" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:49" x14ac:dyDescent="0.2">
       <c r="F29" s="35" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Upgrade FY23 £BOWL projections matching analysts
</commit_message>
<xml_diff>
--- a/Overview - Leisure Facilities.xlsx
+++ b/Overview - Leisure Facilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBEC21D-CD05-4637-8593-52FE9835FE65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D330EE-F751-440A-9D34-26A4AB192440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5EB38F2A-A5E5-4604-9A50-AFDB2AF73DAE}"/>
+    <workbookView xWindow="1950" yWindow="3150" windowWidth="21600" windowHeight="11235" xr2:uid="{5EB38F2A-A5E5-4604-9A50-AFDB2AF73DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -473,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,12 +587,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -611,7 +614,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -711,7 +714,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Screener"/>
@@ -728,8 +731,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -744,7 +750,7 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>2.52</v>
+            <v>2.4350000000000001</v>
           </cell>
         </row>
         <row r="7">
@@ -754,7 +760,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>431.48036987999996</v>
+            <v>416.92646851499995</v>
           </cell>
         </row>
         <row r="11">
@@ -764,7 +770,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>387.33136987999995</v>
+            <v>372.77746851499995</v>
           </cell>
         </row>
         <row r="23">
@@ -802,27 +808,27 @@
         </row>
         <row r="33">
           <cell r="C33">
-            <v>3.0961565002870257</v>
+            <v>2.9917226500789318</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>2.1190470969452901</v>
+            <v>2.0475713020086435</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>1.9022265488655337</v>
+            <v>1.830750753928887</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>13.332662899445351</v>
+            <v>12.882950063551361</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>11.974629625919729</v>
+            <v>11.524685232022494</v>
           </cell>
         </row>
       </sheetData>
@@ -894,7 +900,7 @@
         </row>
         <row r="22">
           <cell r="AP22">
-            <v>2.7033970290475535</v>
+            <v>2.8326737220533205</v>
           </cell>
         </row>
       </sheetData>
@@ -905,7 +911,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1067,7 +1073,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1165,7 +1171,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1234,7 +1240,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1679,7 +1685,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1943,7 +1949,7 @@
       </c>
       <c r="F4" s="12">
         <f>[3]Main!$C$6</f>
-        <v>2.52</v>
+        <v>2.4350000000000001</v>
       </c>
       <c r="G4" s="9">
         <f>[3]Main!$C$7</f>
@@ -1951,7 +1957,7 @@
       </c>
       <c r="H4" s="9">
         <f>[3]Main!$C$8</f>
-        <v>431.48036987999996</v>
+        <v>416.92646851499995</v>
       </c>
       <c r="I4" s="9">
         <f>[3]Main!$C$11</f>
@@ -1959,7 +1965,7 @@
       </c>
       <c r="J4" s="9">
         <f>[3]Main!$C$12</f>
-        <v>387.33136987999995</v>
+        <v>372.77746851499995</v>
       </c>
       <c r="K4" s="2" t="str">
         <f>[3]Main!$C$28</f>
@@ -1975,7 +1981,7 @@
       </c>
       <c r="N4" s="20">
         <f>'[3]Financial Model'!$AP$22</f>
-        <v>2.7033970290475535</v>
+        <v>2.8326737220533205</v>
       </c>
       <c r="O4" s="20">
         <f>'[3]Financial Model'!$AP$16</f>
@@ -1983,23 +1989,23 @@
       </c>
       <c r="Q4" s="10">
         <f>[3]Main!$C$33</f>
-        <v>3.0961565002870257</v>
+        <v>2.9917226500789318</v>
       </c>
       <c r="R4" s="10">
         <f>[3]Main!$C$34</f>
-        <v>2.1190470969452901</v>
+        <v>2.0475713020086435</v>
       </c>
       <c r="S4" s="10">
         <f>[3]Main!$C$35</f>
-        <v>1.9022265488655337</v>
+        <v>1.830750753928887</v>
       </c>
       <c r="T4" s="10">
         <f>[3]Main!$C$36</f>
-        <v>13.332662899445351</v>
+        <v>12.882950063551361</v>
       </c>
       <c r="U4" s="10">
         <f>[3]Main!$C$37</f>
-        <v>11.974629625919729</v>
+        <v>11.524685232022494</v>
       </c>
       <c r="X4" s="14">
         <f>'[3]Financial Model'!$W$12</f>
@@ -2122,11 +2128,11 @@
         <f>[4]Main!$C$12</f>
         <v>390.14732449999997</v>
       </c>
-      <c r="K5" s="40" t="str">
+      <c r="K5" s="2" t="str">
         <f>[4]Main!$C$28</f>
         <v>H123</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="15">
         <f>[4]Main!$D$28</f>
         <v>45189</v>
       </c>
@@ -2717,10 +2723,10 @@
       </c>
     </row>
     <row r="28" spans="2:49" x14ac:dyDescent="0.2">
-      <c r="F28" s="42" t="s">
+      <c r="F28" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="43"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="32" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Update re £TEG takeover rumour
</commit_message>
<xml_diff>
--- a/Overview - Leisure Facilities.xlsx
+++ b/Overview - Leisure Facilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D330EE-F751-440A-9D34-26A4AB192440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7684F41E-554F-4EDD-AF8F-72685BBE525C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="3150" windowWidth="21600" windowHeight="11235" xr2:uid="{5EB38F2A-A5E5-4604-9A50-AFDB2AF73DAE}"/>
   </bookViews>
@@ -28,15 +28,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -614,7 +605,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -714,7 +705,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Screener"/>
@@ -731,11 +722,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -750,7 +738,7 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>2.4350000000000001</v>
+            <v>2.6949999999999998</v>
           </cell>
         </row>
         <row r="7">
@@ -760,7 +748,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>416.92646851499995</v>
+            <v>461.44428445499994</v>
           </cell>
         </row>
         <row r="11">
@@ -770,7 +758,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>372.77746851499995</v>
+            <v>417.29528445499994</v>
           </cell>
         </row>
         <row r="23">
@@ -808,27 +796,27 @@
         </row>
         <row r="33">
           <cell r="C33">
-            <v>2.9917226500789318</v>
+            <v>3.3111673683625136</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>2.0475713020086435</v>
+            <v>2.2662031453442686</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>1.830750753928887</v>
+            <v>2.0493825972645121</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>12.882950063551361</v>
+            <v>14.258542267462389</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>11.524685232022494</v>
+            <v>12.900985731002272</v>
           </cell>
         </row>
       </sheetData>
@@ -875,7 +863,7 @@
         </row>
         <row r="20">
           <cell r="AP20">
-            <v>9.3325605131998355</v>
+            <v>9.9807066989049318</v>
           </cell>
         </row>
         <row r="21">
@@ -900,7 +888,7 @@
         </row>
         <row r="22">
           <cell r="AP22">
-            <v>2.8326737220533205</v>
+            <v>2.7034162148070249</v>
           </cell>
         </row>
       </sheetData>
@@ -911,7 +899,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -926,7 +914,7 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>2.75</v>
+            <v>3.1</v>
           </cell>
         </row>
         <row r="7">
@@ -936,7 +924,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>188.36432449999998</v>
+            <v>212.33796580000001</v>
           </cell>
         </row>
         <row r="11">
@@ -946,7 +934,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>390.14732449999997</v>
+            <v>414.12096580000002</v>
           </cell>
         </row>
         <row r="23">
@@ -979,27 +967,27 @@
         </row>
         <row r="33">
           <cell r="C33">
-            <v>2.8119534312627823</v>
+            <v>3.1698384134235003</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>1.4632398140308083</v>
+            <v>1.6494703358165479</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>3.0307177331023607</v>
+            <v>3.2169482548881003</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>9.1425678056593718</v>
+            <v>10.306167344561473</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>18.93643277678008</v>
+            <v>20.100032315682185</v>
           </cell>
         </row>
       </sheetData>
@@ -1073,7 +1061,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1171,7 +1159,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1240,7 +1228,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -1682,10 +1670,10 @@
   <dimension ref="B2:AW29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1949,7 +1937,7 @@
       </c>
       <c r="F4" s="12">
         <f>[3]Main!$C$6</f>
-        <v>2.4350000000000001</v>
+        <v>2.6949999999999998</v>
       </c>
       <c r="G4" s="9">
         <f>[3]Main!$C$7</f>
@@ -1957,7 +1945,7 @@
       </c>
       <c r="H4" s="9">
         <f>[3]Main!$C$8</f>
-        <v>416.92646851499995</v>
+        <v>461.44428445499994</v>
       </c>
       <c r="I4" s="9">
         <f>[3]Main!$C$11</f>
@@ -1965,7 +1953,7 @@
       </c>
       <c r="J4" s="9">
         <f>[3]Main!$C$12</f>
-        <v>372.77746851499995</v>
+        <v>417.29528445499994</v>
       </c>
       <c r="K4" s="2" t="str">
         <f>[3]Main!$C$28</f>
@@ -1977,11 +1965,11 @@
       </c>
       <c r="M4" s="19">
         <f>'[3]Financial Model'!$AP$20</f>
-        <v>9.3325605131998355</v>
+        <v>9.9807066989049318</v>
       </c>
       <c r="N4" s="20">
         <f>'[3]Financial Model'!$AP$22</f>
-        <v>2.8326737220533205</v>
+        <v>2.7034162148070249</v>
       </c>
       <c r="O4" s="20">
         <f>'[3]Financial Model'!$AP$16</f>
@@ -1989,23 +1977,23 @@
       </c>
       <c r="Q4" s="10">
         <f>[3]Main!$C$33</f>
-        <v>2.9917226500789318</v>
+        <v>3.3111673683625136</v>
       </c>
       <c r="R4" s="10">
         <f>[3]Main!$C$34</f>
-        <v>2.0475713020086435</v>
+        <v>2.2662031453442686</v>
       </c>
       <c r="S4" s="10">
         <f>[3]Main!$C$35</f>
-        <v>1.830750753928887</v>
+        <v>2.0493825972645121</v>
       </c>
       <c r="T4" s="10">
         <f>[3]Main!$C$36</f>
-        <v>12.882950063551361</v>
+        <v>14.258542267462389</v>
       </c>
       <c r="U4" s="10">
         <f>[3]Main!$C$37</f>
-        <v>11.524685232022494</v>
+        <v>12.900985731002272</v>
       </c>
       <c r="X4" s="14">
         <f>'[3]Financial Model'!$W$12</f>
@@ -2110,7 +2098,7 @@
       </c>
       <c r="F5" s="12">
         <f>[4]Main!$C$6</f>
-        <v>2.75</v>
+        <v>3.1</v>
       </c>
       <c r="G5" s="9">
         <f>[4]Main!$C$7</f>
@@ -2118,7 +2106,7 @@
       </c>
       <c r="H5" s="9">
         <f>[4]Main!$C$8</f>
-        <v>188.36432449999998</v>
+        <v>212.33796580000001</v>
       </c>
       <c r="I5" s="9">
         <f>[4]Main!$C$11</f>
@@ -2126,7 +2114,7 @@
       </c>
       <c r="J5" s="9">
         <f>[4]Main!$C$12</f>
-        <v>390.14732449999997</v>
+        <v>414.12096580000002</v>
       </c>
       <c r="K5" s="2" t="str">
         <f>[4]Main!$C$28</f>
@@ -2138,23 +2126,23 @@
       </c>
       <c r="Q5" s="10">
         <f>[4]Main!$C$33</f>
-        <v>2.8119534312627823</v>
+        <v>3.1698384134235003</v>
       </c>
       <c r="R5" s="10">
         <f>[4]Main!$C$34</f>
-        <v>1.4632398140308083</v>
+        <v>1.6494703358165479</v>
       </c>
       <c r="S5" s="10">
         <f>[4]Main!$C$35</f>
-        <v>3.0307177331023607</v>
+        <v>3.2169482548881003</v>
       </c>
       <c r="T5" s="10">
         <f>[4]Main!$C$36</f>
-        <v>9.1425678056593718</v>
+        <v>10.306167344561473</v>
       </c>
       <c r="U5" s="10">
         <f>[4]Main!$C$37</f>
-        <v>18.93643277678008</v>
+        <v>20.100032315682185</v>
       </c>
       <c r="X5" s="14">
         <f>'[4]Financial Model'!$V$19</f>

</xml_diff>